<commit_message>
preparation col box mod server test
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -158,12 +158,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,8 +206,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,7 +235,7 @@
   <dimension ref="B1:Q42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1042,7 +1052,7 @@
       <c r="J38" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="0" t="s">
+      <c r="K38" s="1" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="0" t="n">

</xml_diff>

<commit_message>
docstring documentation config.py generation_SIP_ensemble.py
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Col box mod" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
   <si>
     <t xml:space="preserve">Main Sims</t>
   </si>
@@ -125,6 +126,21 @@
   </si>
   <si>
     <t xml:space="preserve">Long kernel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golovin:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kappa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only to seed 1243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only to seed 1227</t>
   </si>
 </sst>
 </file>
@@ -234,8 +250,8 @@
   </sheetPr>
   <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1120,4 +1136,165 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="C6:I17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.5"/>
+  </cols>
+  <sheetData>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docstring docum. integration.py INWORK
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t xml:space="preserve">Main Sims</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">only to seed 1227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000, 2000</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
   </sheetPr>
   <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -1143,17 +1146,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:I17"/>
+  <dimension ref="B6:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,6 +1289,50 @@
         <v>3000</v>
       </c>
       <c r="H17" s="0" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="0" t="n">
         <v>3000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bugfix generate_plot_data wo_collision file name
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
   <si>
     <t xml:space="preserve">Main Sims</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t xml:space="preserve">Long kernel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTS 15.04.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecol const 0.5</t>
   </si>
   <si>
     <t xml:space="preserve">Golovin:</t>
@@ -236,12 +242,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -251,15 +257,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:Q42"/>
+  <dimension ref="B1:Q52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M35" activeCellId="0" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.53"/>
@@ -1130,6 +1137,202 @@
         <v>34</v>
       </c>
     </row>
+    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M46" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2001</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M49" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3001</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1148,8 +1351,8 @@
   </sheetPr>
   <dimension ref="B6:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1162,7 +1365,7 @@
   <sheetData>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>17</v>
@@ -1173,13 +1376,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,13 +1456,13 @@
         <v>400</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>400</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,13 +1470,13 @@
         <v>1000</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,7 +1503,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,7 +1525,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
axis labels subscripts upright
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -257,18 +257,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:Q52"/>
+  <dimension ref="B1:Q51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M35" activeCellId="0" sqref="M35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M51" activeCellId="0" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="10.73"/>
   </cols>
@@ -1261,10 +1261,10 @@
         <v>3</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>1001</v>
+        <v>3001</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>1001</v>
+        <v>3001</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>75</v>
@@ -1282,10 +1282,10 @@
         <v>15</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L49" s="0" t="n">
         <v>60</v>
@@ -1299,10 +1299,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>3001</v>
+        <v>1001</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>3001</v>
+        <v>1001</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>75</v>
@@ -1320,10 +1320,10 @@
         <v>15</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L50" s="0" t="n">
         <v>60</v>
@@ -1332,6 +1332,7 @@
         <v>40</v>
       </c>
     </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1351,7 +1352,7 @@
   </sheetPr>
   <dimension ref="B6:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
generate_plot_data.py: also copy sim logs
</commit_message>
<xml_diff>
--- a/NOTES/job_table.xlsx
+++ b/NOTES/job_table.xlsx
@@ -259,8 +259,8 @@
   </sheetPr>
   <dimension ref="B1:Q51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M51" activeCellId="0" sqref="M51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>